<commit_message>
Added filters and line crossings
</commit_message>
<xml_diff>
--- a/Data/Excels/KITS_RFQ_template.xlsx
+++ b/Data/Excels/KITS_RFQ_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AHMED Raja\Desktop\XINLIDA\Web app v3\Data\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AHMED Raja\Desktop\XINLIDA\Web app v4\Data\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF270776-8EFA-47CF-9DF8-1D46FFE505A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35673F3-CBB9-4068-83B6-D1FCF0DF369C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0BCD3FCC-ADED-4DA8-AE61-4BD9FE047C9C}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>D Plate Number</t>
   </si>
   <si>
-    <t>D914</t>
-  </si>
-  <si>
     <t>D430, D1047, D815E</t>
   </si>
   <si>
@@ -56,7 +53,10 @@
     <t>D787</t>
   </si>
   <si>
-    <t>D1159</t>
+    <t>D5555</t>
+  </si>
+  <si>
+    <t>D00914</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,32 +426,32 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>